<commit_message>
Working on Dark mode
</commit_message>
<xml_diff>
--- a/Colors.xlsx
+++ b/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\videomedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D28536-C1A6-47C5-A0AD-399C405BC95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B936CBE2-97D9-48CB-A47A-E05256DC9EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3CF810E2-6665-4786-8465-095BA01D6E4F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Electric Blue</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>#C0C0C0</t>
+  </si>
+  <si>
+    <t>#D2691E</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
   <dimension ref="A7:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,6 +612,9 @@
       <c r="K19" t="s">
         <v>5</v>
       </c>
+      <c r="L19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I21" s="10" t="s">

</xml_diff>